<commit_message>
Plot figures, and experiments on new data set 2023-08-08
</commit_message>
<xml_diff>
--- a/result/Sensitivity_KF_measure.xlsx
+++ b/result/Sensitivity_KF_measure.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduSyncdisk\Study\【0】博士研究方向\【1】Kalman Filter\Kalman_filter_sensor_drift\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\BaiduSyncdisk\Study\【0】博士研究方向\【1】Kalman Filter\Kalman_filter_sensor_drift\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8B6B88-F403-41FE-A158-E297B9013229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE39C57-7E4C-443F-97C2-D15528F0BDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="145C" sheetId="1" r:id="rId1"/>
+    <sheet name="140C" sheetId="2" r:id="rId2"/>
+    <sheet name="135C" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,12 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>145C</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,6 +58,14 @@
   </si>
   <si>
     <t>std</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>140C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>135C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -387,12 +395,12 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -444,7 +452,7 @@
         <v>5.4039999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>6.3179999999999996</v>
       </c>
@@ -467,7 +475,7 @@
         <v>5.4219999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>6.0259999999999998</v>
       </c>
@@ -490,7 +498,7 @@
         <v>6.1159999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>7.1550000000000002</v>
       </c>
@@ -513,7 +521,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5.6310000000000002</v>
       </c>
@@ -536,7 +544,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6.5419999999999998</v>
       </c>
@@ -559,7 +567,7 @@
         <v>5.3929999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5.8769999999999998</v>
       </c>
@@ -582,7 +590,7 @@
         <v>4.6379999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5.7729999999999997</v>
       </c>
@@ -605,7 +613,7 @@
         <v>6.1630000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6.65</v>
       </c>
@@ -628,7 +636,7 @@
         <v>7.0789999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>5.7910000000000004</v>
       </c>
@@ -651,7 +659,7 @@
         <v>6.6520000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -684,7 +692,7 @@
         <v>5.8687000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -717,7 +725,7 @@
         <v>0.75863664996272084</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -743,7 +751,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>28.48</v>
       </c>
@@ -766,7 +774,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>26.02</v>
       </c>
@@ -789,7 +797,7 @@
         <v>27.96</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>31.22</v>
       </c>
@@ -812,7 +820,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>25.35</v>
       </c>
@@ -835,7 +843,7 @@
         <v>22.54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>27.94</v>
       </c>
@@ -858,7 +866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>25.82</v>
       </c>
@@ -881,7 +889,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>24.12</v>
       </c>
@@ -904,7 +912,7 @@
         <v>26.56</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>30.04</v>
       </c>
@@ -927,7 +935,7 @@
         <v>31.58</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24.36</v>
       </c>
@@ -950,7 +958,7 @@
         <v>30.78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -983,7 +991,7 @@
         <v>26.45</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1014,6 +1022,1023 @@
       <c r="H27">
         <f t="shared" si="3"/>
         <v>3.5284557528754874</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7337C89-B08E-4CC5-81D8-8A86300B343D}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>25</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>35</v>
+      </c>
+      <c r="F1">
+        <v>40</v>
+      </c>
+      <c r="G1">
+        <v>45</v>
+      </c>
+      <c r="H1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>9.3960000000000008</v>
+      </c>
+      <c r="C2">
+        <v>7.7619999999999996</v>
+      </c>
+      <c r="D2">
+        <v>8.61</v>
+      </c>
+      <c r="E2">
+        <v>7.5960000000000001</v>
+      </c>
+      <c r="F2">
+        <v>6.2380000000000004</v>
+      </c>
+      <c r="G2">
+        <v>6.2969999999999997</v>
+      </c>
+      <c r="H2">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>6.8460000000000001</v>
+      </c>
+      <c r="C3">
+        <v>7.8390000000000004</v>
+      </c>
+      <c r="D3">
+        <v>7.47</v>
+      </c>
+      <c r="E3">
+        <v>6.4720000000000004</v>
+      </c>
+      <c r="F3">
+        <v>7.3869999999999996</v>
+      </c>
+      <c r="G3">
+        <v>7.9409999999999998</v>
+      </c>
+      <c r="H3">
+        <v>6.819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>7.7930000000000001</v>
+      </c>
+      <c r="C4">
+        <v>6.8710000000000004</v>
+      </c>
+      <c r="D4">
+        <v>7.0190000000000001</v>
+      </c>
+      <c r="E4">
+        <v>6.1310000000000002</v>
+      </c>
+      <c r="F4">
+        <v>6.4669999999999996</v>
+      </c>
+      <c r="G4">
+        <v>8.6929999999999996</v>
+      </c>
+      <c r="H4">
+        <v>7.782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>8.452</v>
+      </c>
+      <c r="C5">
+        <v>9.4990000000000006</v>
+      </c>
+      <c r="D5">
+        <v>7.0250000000000004</v>
+      </c>
+      <c r="E5">
+        <v>7.2750000000000004</v>
+      </c>
+      <c r="F5">
+        <v>6.5839999999999996</v>
+      </c>
+      <c r="G5">
+        <v>6.48</v>
+      </c>
+      <c r="H5">
+        <v>6.4669999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.6120000000000001</v>
+      </c>
+      <c r="C6">
+        <v>7.5339999999999998</v>
+      </c>
+      <c r="D6">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="E6">
+        <v>6.83</v>
+      </c>
+      <c r="F6">
+        <v>6.5469999999999997</v>
+      </c>
+      <c r="G6">
+        <v>5.9770000000000003</v>
+      </c>
+      <c r="H6">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>8.6620000000000008</v>
+      </c>
+      <c r="C7">
+        <v>8.7490000000000006</v>
+      </c>
+      <c r="D7">
+        <v>8.1359999999999992</v>
+      </c>
+      <c r="E7">
+        <v>6.5640000000000001</v>
+      </c>
+      <c r="F7">
+        <v>6.1769999999999996</v>
+      </c>
+      <c r="G7">
+        <v>7.0869999999999997</v>
+      </c>
+      <c r="H7">
+        <v>6.8840000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>9.0429999999999993</v>
+      </c>
+      <c r="C8">
+        <v>6.9870000000000001</v>
+      </c>
+      <c r="D8">
+        <v>7.7069999999999999</v>
+      </c>
+      <c r="E8">
+        <v>6.492</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7.4580000000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6.1779999999999999</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7.2539999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8.6910000000000007</v>
+      </c>
+      <c r="C9">
+        <v>7.79</v>
+      </c>
+      <c r="D9">
+        <v>7.923</v>
+      </c>
+      <c r="E9">
+        <v>7.5430000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7.7779999999999996</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7.4370000000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6.4429999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6.8929999999999998</v>
+      </c>
+      <c r="C10">
+        <v>7.9379999999999997</v>
+      </c>
+      <c r="D10">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="E10">
+        <v>8.4789999999999992</v>
+      </c>
+      <c r="F10" s="1">
+        <v>7.5490000000000004</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.52</v>
+      </c>
+      <c r="H10" s="1">
+        <v>7.165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8.5169999999999995</v>
+      </c>
+      <c r="C11">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="D11">
+        <v>7.984</v>
+      </c>
+      <c r="E11">
+        <v>6.28</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7.5019999999999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.782</v>
+      </c>
+      <c r="H11" s="1">
+        <v>6.5659999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>30.09</v>
+      </c>
+      <c r="C16">
+        <v>26.96</v>
+      </c>
+      <c r="D16">
+        <v>29.4</v>
+      </c>
+      <c r="E16">
+        <v>26.29</v>
+      </c>
+      <c r="F16">
+        <v>20.71</v>
+      </c>
+      <c r="G16">
+        <v>21.55</v>
+      </c>
+      <c r="H16">
+        <v>23.18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>23.72</v>
+      </c>
+      <c r="C17">
+        <v>26.27</v>
+      </c>
+      <c r="D17">
+        <v>24.68</v>
+      </c>
+      <c r="E17">
+        <v>21.82</v>
+      </c>
+      <c r="F17">
+        <v>24.62</v>
+      </c>
+      <c r="G17">
+        <v>26.96</v>
+      </c>
+      <c r="H17">
+        <v>23.12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>24.11</v>
+      </c>
+      <c r="C18">
+        <v>23.69</v>
+      </c>
+      <c r="D18">
+        <v>23.95</v>
+      </c>
+      <c r="E18">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="F18">
+        <v>22.92</v>
+      </c>
+      <c r="G18">
+        <v>29.57</v>
+      </c>
+      <c r="H18">
+        <v>25.76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>28.39</v>
+      </c>
+      <c r="C19">
+        <v>32.64</v>
+      </c>
+      <c r="D19">
+        <v>24.25</v>
+      </c>
+      <c r="E19">
+        <v>24.25</v>
+      </c>
+      <c r="F19">
+        <v>22.6</v>
+      </c>
+      <c r="G19">
+        <v>21.18</v>
+      </c>
+      <c r="H19">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>25.02</v>
+      </c>
+      <c r="C20">
+        <v>25.36</v>
+      </c>
+      <c r="D20">
+        <v>25.94</v>
+      </c>
+      <c r="E20">
+        <v>22.78</v>
+      </c>
+      <c r="F20">
+        <v>21.3</v>
+      </c>
+      <c r="G20">
+        <v>20.91</v>
+      </c>
+      <c r="H20">
+        <v>21.56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>28.82</v>
+      </c>
+      <c r="C21">
+        <v>29.17</v>
+      </c>
+      <c r="D21">
+        <v>26.95</v>
+      </c>
+      <c r="E21">
+        <v>21.59</v>
+      </c>
+      <c r="F21">
+        <v>20.9</v>
+      </c>
+      <c r="G21">
+        <v>24.89</v>
+      </c>
+      <c r="H21">
+        <v>23.28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>28.96</v>
+      </c>
+      <c r="C22">
+        <v>25.17</v>
+      </c>
+      <c r="D22">
+        <v>24.1</v>
+      </c>
+      <c r="E22">
+        <v>21.79</v>
+      </c>
+      <c r="F22">
+        <v>25.29</v>
+      </c>
+      <c r="G22">
+        <v>20.76</v>
+      </c>
+      <c r="H22">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>28.34</v>
+      </c>
+      <c r="C23">
+        <v>25.44</v>
+      </c>
+      <c r="D23">
+        <v>25.65</v>
+      </c>
+      <c r="E23">
+        <v>25.28</v>
+      </c>
+      <c r="F23">
+        <v>26.94</v>
+      </c>
+      <c r="G23">
+        <v>25.15</v>
+      </c>
+      <c r="H23">
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23.08</v>
+      </c>
+      <c r="C24">
+        <v>26.68</v>
+      </c>
+      <c r="D24">
+        <v>19.48</v>
+      </c>
+      <c r="E24">
+        <v>27.83</v>
+      </c>
+      <c r="F24">
+        <v>24.49</v>
+      </c>
+      <c r="G24">
+        <v>22.26</v>
+      </c>
+      <c r="H24">
+        <v>24.79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>26.07</v>
+      </c>
+      <c r="C25">
+        <v>25.41</v>
+      </c>
+      <c r="D25">
+        <v>26.35</v>
+      </c>
+      <c r="E25">
+        <v>22.29</v>
+      </c>
+      <c r="F25">
+        <v>24.68</v>
+      </c>
+      <c r="G25">
+        <v>22.46</v>
+      </c>
+      <c r="H25">
+        <v>21.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D913C1A0-B1D8-4086-A907-EF8FD85BD55F}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>25</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>35</v>
+      </c>
+      <c r="F1">
+        <v>40</v>
+      </c>
+      <c r="G1">
+        <v>45</v>
+      </c>
+      <c r="H1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="C2">
+        <v>7.7</v>
+      </c>
+      <c r="D2">
+        <v>6.7480000000000002</v>
+      </c>
+      <c r="E2">
+        <v>7.3289999999999997</v>
+      </c>
+      <c r="F2">
+        <v>6.2510000000000003</v>
+      </c>
+      <c r="G2">
+        <v>6.7009999999999996</v>
+      </c>
+      <c r="H2">
+        <v>8.3309999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>8.577</v>
+      </c>
+      <c r="C3">
+        <v>7.798</v>
+      </c>
+      <c r="D3">
+        <v>7.3339999999999996</v>
+      </c>
+      <c r="E3">
+        <v>8.7590000000000003</v>
+      </c>
+      <c r="F3">
+        <v>7.8849999999999998</v>
+      </c>
+      <c r="G3">
+        <v>7.0679999999999996</v>
+      </c>
+      <c r="H3">
+        <v>6.8730000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>7.4279999999999999</v>
+      </c>
+      <c r="C4">
+        <v>8.1349999999999998</v>
+      </c>
+      <c r="D4">
+        <v>8.0139999999999993</v>
+      </c>
+      <c r="E4">
+        <v>6.4470000000000001</v>
+      </c>
+      <c r="F4">
+        <v>6.9420000000000002</v>
+      </c>
+      <c r="G4">
+        <v>8.0429999999999993</v>
+      </c>
+      <c r="H4">
+        <v>6.3150000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.7430000000000003</v>
+      </c>
+      <c r="C5">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D5">
+        <v>6.96</v>
+      </c>
+      <c r="E5">
+        <v>6.7439999999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.6260000000000003</v>
+      </c>
+      <c r="G5">
+        <v>6.1559999999999997</v>
+      </c>
+      <c r="H5">
+        <v>6.1539999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>8.5329999999999995</v>
+      </c>
+      <c r="C6">
+        <v>9.4030000000000005</v>
+      </c>
+      <c r="D6">
+        <v>7.194</v>
+      </c>
+      <c r="E6">
+        <v>6.9279999999999999</v>
+      </c>
+      <c r="F6">
+        <v>6.681</v>
+      </c>
+      <c r="G6">
+        <v>8.4380000000000006</v>
+      </c>
+      <c r="H6">
+        <v>7.2720000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>9.2629999999999999</v>
+      </c>
+      <c r="C7">
+        <v>8.2010000000000005</v>
+      </c>
+      <c r="D7">
+        <v>6.9889999999999999</v>
+      </c>
+      <c r="E7">
+        <v>7.351</v>
+      </c>
+      <c r="F7">
+        <v>6.6130000000000004</v>
+      </c>
+      <c r="G7">
+        <v>7.2549999999999999</v>
+      </c>
+      <c r="H7">
+        <v>7.6059999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6.5369999999999999</v>
+      </c>
+      <c r="C8">
+        <v>7.4969999999999999</v>
+      </c>
+      <c r="D8">
+        <v>5.8769999999999998</v>
+      </c>
+      <c r="E8">
+        <v>7.3140000000000001</v>
+      </c>
+      <c r="F8">
+        <v>7.5339999999999998</v>
+      </c>
+      <c r="G8">
+        <v>8.5519999999999996</v>
+      </c>
+      <c r="H8">
+        <v>6.8959999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8.5050000000000008</v>
+      </c>
+      <c r="C9">
+        <v>6.5709999999999997</v>
+      </c>
+      <c r="D9">
+        <v>7.6109999999999998</v>
+      </c>
+      <c r="E9">
+        <v>7.7060000000000004</v>
+      </c>
+      <c r="F9">
+        <v>6.8419999999999996</v>
+      </c>
+      <c r="G9">
+        <v>6.7480000000000002</v>
+      </c>
+      <c r="H9">
+        <v>6.5839999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8.6980000000000004</v>
+      </c>
+      <c r="C10">
+        <v>7.2809999999999997</v>
+      </c>
+      <c r="D10">
+        <v>7.3860000000000001</v>
+      </c>
+      <c r="E10">
+        <v>6.8760000000000003</v>
+      </c>
+      <c r="F10">
+        <v>7.7309999999999999</v>
+      </c>
+      <c r="G10">
+        <v>6.9939999999999998</v>
+      </c>
+      <c r="H10">
+        <v>6.0069999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8.2349999999999994</v>
+      </c>
+      <c r="C11">
+        <v>7.0759999999999996</v>
+      </c>
+      <c r="D11">
+        <v>7.407</v>
+      </c>
+      <c r="E11">
+        <v>6.5529999999999999</v>
+      </c>
+      <c r="F11">
+        <v>6.9320000000000004</v>
+      </c>
+      <c r="G11">
+        <v>7.093</v>
+      </c>
+      <c r="H11">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>27.14</v>
+      </c>
+      <c r="C16">
+        <v>23.91</v>
+      </c>
+      <c r="D16">
+        <v>22.43</v>
+      </c>
+      <c r="E16">
+        <v>24.54</v>
+      </c>
+      <c r="F16">
+        <v>20.6</v>
+      </c>
+      <c r="G16">
+        <v>22.11</v>
+      </c>
+      <c r="H16">
+        <v>27.35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>29.48</v>
+      </c>
+      <c r="C17">
+        <v>25.75</v>
+      </c>
+      <c r="D17">
+        <v>23.47</v>
+      </c>
+      <c r="E17">
+        <v>26.93</v>
+      </c>
+      <c r="F17">
+        <v>25.36</v>
+      </c>
+      <c r="G17">
+        <v>22.96</v>
+      </c>
+      <c r="H17">
+        <v>21.85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>24.12</v>
+      </c>
+      <c r="C18">
+        <v>26.51</v>
+      </c>
+      <c r="D18">
+        <v>25.87</v>
+      </c>
+      <c r="E18">
+        <v>20.75</v>
+      </c>
+      <c r="F18">
+        <v>22.34</v>
+      </c>
+      <c r="G18">
+        <v>25.66</v>
+      </c>
+      <c r="H18">
+        <v>19.89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>24.65</v>
+      </c>
+      <c r="C19">
+        <v>25.32</v>
+      </c>
+      <c r="D19">
+        <v>23.97</v>
+      </c>
+      <c r="E19">
+        <v>22.68</v>
+      </c>
+      <c r="F19">
+        <v>25.46</v>
+      </c>
+      <c r="G19">
+        <v>19.48</v>
+      </c>
+      <c r="H19">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>27.23</v>
+      </c>
+      <c r="C20">
+        <v>28.6</v>
+      </c>
+      <c r="D20">
+        <v>22.86</v>
+      </c>
+      <c r="E20">
+        <v>23.26</v>
+      </c>
+      <c r="F20">
+        <v>22.06</v>
+      </c>
+      <c r="G20">
+        <v>27.58</v>
+      </c>
+      <c r="H20">
+        <v>24.08</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>26.58</v>
+      </c>
+      <c r="D21">
+        <v>22.58</v>
+      </c>
+      <c r="E21">
+        <v>23.45</v>
+      </c>
+      <c r="F21">
+        <v>22.13</v>
+      </c>
+      <c r="G21">
+        <v>24.94</v>
+      </c>
+      <c r="H21">
+        <v>25.37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21.33</v>
+      </c>
+      <c r="C22">
+        <v>25.46</v>
+      </c>
+      <c r="D22">
+        <v>19.57</v>
+      </c>
+      <c r="E22">
+        <v>23.6</v>
+      </c>
+      <c r="F22">
+        <v>24.96</v>
+      </c>
+      <c r="G22">
+        <v>28.38</v>
+      </c>
+      <c r="H22">
+        <v>22.27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>26.79</v>
+      </c>
+      <c r="C23">
+        <v>21.98</v>
+      </c>
+      <c r="D23">
+        <v>25.39</v>
+      </c>
+      <c r="E23">
+        <v>24.93</v>
+      </c>
+      <c r="F23">
+        <v>22.38</v>
+      </c>
+      <c r="G23">
+        <v>21.97</v>
+      </c>
+      <c r="H23">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>28.56</v>
+      </c>
+      <c r="C24">
+        <v>23.37</v>
+      </c>
+      <c r="D24">
+        <v>24.41</v>
+      </c>
+      <c r="E24">
+        <v>20.38</v>
+      </c>
+      <c r="F24">
+        <v>25.5</v>
+      </c>
+      <c r="G24">
+        <v>21.86</v>
+      </c>
+      <c r="H24">
+        <v>19.41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>27.64</v>
+      </c>
+      <c r="C25">
+        <v>23.09</v>
+      </c>
+      <c r="D25">
+        <v>22.39</v>
+      </c>
+      <c r="E25">
+        <v>22.22</v>
+      </c>
+      <c r="F25">
+        <v>22.22</v>
+      </c>
+      <c r="G25">
+        <v>22.98</v>
+      </c>
+      <c r="H25">
+        <v>20.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>